<commit_message>
Clean up json generators that it'll generate from xlsx file instead of CSV
</commit_message>
<xml_diff>
--- a/bus_stops.xlsx
+++ b/bus_stops.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seankzw/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seankzw/Desktop/SIT/Y1T2/csc1108/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA8EC6E-8CF1-8148-BA1F-59AF038AF43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7E69C7-55CC-3547-A53D-20659FE6727C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="9" xr2:uid="{F10A9419-1CB3-714B-AE05-C7B58E3111EF}"/>
+    <workbookView xWindow="7060" yWindow="760" windowWidth="23180" windowHeight="18880" activeTab="9" xr2:uid="{F10A9419-1CB3-714B-AE05-C7B58E3111EF}"/>
   </bookViews>
   <sheets>
     <sheet name="P101-loop" sheetId="1" r:id="rId1"/>
@@ -1440,7 +1440,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1680,7 +1680,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1975,7 +1975,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3351,7 +3351,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B2" sqref="B2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3689,8 +3689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09611D23-CBEC-BB47-8C1C-593243700395}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Json should be done
</commit_message>
<xml_diff>
--- a/bus_stops.xlsx
+++ b/bus_stops.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seankzw/Desktop/SIT/Y1T2/csc1108/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36566917-9DE6-6844-A855-5D06298828B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFE9224-1F3F-D645-9CEA-0E13E8B2C252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="8" xr2:uid="{F10A9419-1CB3-714B-AE05-C7B58E3111EF}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F10A9419-1CB3-714B-AE05-C7B58E3111EF}"/>
   </bookViews>
   <sheets>
     <sheet name="P101-loop" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>1.4627466510403129, 103.73965194475493</t>
   </si>
   <si>
-    <t>Maktab Sultan Abu Bakar (English College</t>
-  </si>
-  <si>
     <t>Hospital Sultanah Aminah</t>
   </si>
   <si>
@@ -1083,6 +1080,9 @@
   </si>
   <si>
     <t>0,0</t>
+  </si>
+  <si>
+    <t>Maktab Sultan Abu Bakar (English College)</t>
   </si>
 </sst>
 </file>
@@ -1436,8 +1436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B383786-A1E5-0A42-A2B9-65DCA6F0CA76}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1448,7 +1448,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1462,7 +1462,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1476,7 +1476,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1506,10 +1506,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1517,7 +1517,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>341</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -1528,10 +1528,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1539,10 +1539,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1550,10 +1550,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1561,10 +1561,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1572,10 +1572,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1583,10 +1583,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1594,10 +1594,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1605,10 +1605,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1616,10 +1616,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1627,10 +1627,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1638,10 +1638,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1649,10 +1649,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1660,7 +1660,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -1689,7 +1689,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1703,10 +1703,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1714,10 +1714,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1725,10 +1725,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1736,10 +1736,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1747,10 +1747,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1758,10 +1758,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1769,10 +1769,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1780,10 +1780,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1791,10 +1791,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1802,10 +1802,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1813,10 +1813,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1824,10 +1824,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1835,10 +1835,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1846,10 +1846,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1857,10 +1857,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1868,10 +1868,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1879,10 +1879,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1890,10 +1890,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1901,10 +1901,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1912,10 +1912,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1923,10 +1923,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1934,10 +1934,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1945,10 +1945,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C24" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1956,10 +1956,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -1984,7 +1984,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1998,10 +1998,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2009,10 +2009,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2020,10 +2020,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2031,10 +2031,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2042,10 +2042,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2053,10 +2053,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2064,10 +2064,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2075,10 +2075,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2086,10 +2086,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2114,7 +2114,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2128,10 +2128,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2139,10 +2139,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2150,10 +2150,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2161,10 +2161,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2172,10 +2172,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2183,10 +2183,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2194,10 +2194,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2205,10 +2205,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2216,10 +2216,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2227,10 +2227,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2238,10 +2238,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2249,10 +2249,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2277,7 +2277,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2291,10 +2291,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2302,10 +2302,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2313,10 +2313,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2324,10 +2324,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2335,10 +2335,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2346,10 +2346,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2357,10 +2357,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2368,10 +2368,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2379,10 +2379,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2390,10 +2390,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2401,10 +2401,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2412,10 +2412,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2423,10 +2423,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2434,10 +2434,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2445,10 +2445,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2456,10 +2456,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2467,10 +2467,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2478,10 +2478,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2489,10 +2489,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2500,10 +2500,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2511,10 +2511,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2522,10 +2522,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2533,10 +2533,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2544,10 +2544,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2555,10 +2555,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2566,10 +2566,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2577,10 +2577,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2588,10 +2588,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2599,10 +2599,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2610,10 +2610,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2621,10 +2621,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2632,10 +2632,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2643,10 +2643,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2654,10 +2654,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2682,7 +2682,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2696,10 +2696,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2707,10 +2707,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2718,10 +2718,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2729,10 +2729,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2740,10 +2740,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2751,10 +2751,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2762,10 +2762,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2773,10 +2773,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2784,10 +2784,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2795,10 +2795,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2806,10 +2806,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2817,10 +2817,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2828,10 +2828,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2839,10 +2839,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2850,10 +2850,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2861,10 +2861,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2872,10 +2872,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2883,10 +2883,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2894,10 +2894,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2905,10 +2905,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2916,10 +2916,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2927,10 +2927,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2938,10 +2938,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2949,10 +2949,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2960,10 +2960,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2971,10 +2971,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2982,10 +2982,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2993,10 +2993,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3004,10 +3004,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -3015,10 +3015,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3043,7 +3043,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3057,10 +3057,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3068,10 +3068,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3079,10 +3079,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3090,10 +3090,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3101,10 +3101,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -3112,10 +3112,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -3123,10 +3123,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -3134,10 +3134,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -3145,10 +3145,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -3156,10 +3156,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -3167,10 +3167,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -3178,10 +3178,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -3189,10 +3189,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -3200,10 +3200,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -3211,10 +3211,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3222,10 +3222,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3233,10 +3233,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3244,10 +3244,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3255,10 +3255,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3266,10 +3266,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3277,10 +3277,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3288,10 +3288,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C23" t="s">
         <v>221</v>
-      </c>
-      <c r="C23" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3299,10 +3299,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C24" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3310,10 +3310,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3321,10 +3321,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3332,7 +3332,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -3361,7 +3361,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3375,7 +3375,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -3389,7 +3389,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3397,10 +3397,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3408,10 +3408,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3419,10 +3419,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -3430,10 +3430,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -3441,10 +3441,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -3452,10 +3452,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -3463,10 +3463,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -3474,10 +3474,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -3485,10 +3485,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -3496,10 +3496,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -3507,10 +3507,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -3518,10 +3518,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -3529,10 +3529,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3540,10 +3540,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3551,10 +3551,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3562,10 +3562,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3573,10 +3573,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3584,10 +3584,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3595,10 +3595,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3606,10 +3606,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3617,10 +3617,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3628,10 +3628,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3639,10 +3639,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3650,10 +3650,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3661,10 +3661,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3672,10 +3672,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3700,7 +3700,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3714,10 +3714,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3725,10 +3725,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3736,10 +3736,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3747,10 +3747,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3758,10 +3758,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -3769,10 +3769,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -3780,10 +3780,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -3791,10 +3791,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -3802,10 +3802,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -3813,10 +3813,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -3824,10 +3824,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -3835,10 +3835,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -3846,10 +3846,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -3857,10 +3857,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -3868,10 +3868,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3879,10 +3879,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3890,10 +3890,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3901,10 +3901,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C19" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3912,10 +3912,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3923,10 +3923,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3934,10 +3934,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3945,10 +3945,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3956,10 +3956,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3967,10 +3967,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3978,10 +3978,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3989,10 +3989,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -4000,10 +4000,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>220</v>
+      </c>
+      <c r="C28" t="s">
         <v>221</v>
-      </c>
-      <c r="C28" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -4011,10 +4011,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -4022,10 +4022,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C30" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -4033,10 +4033,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C31" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -4044,7 +4044,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
@@ -4060,7 +4060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0A68FDA-B711-404A-BB23-6CDB140930DB}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -4072,7 +4072,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -4086,7 +4086,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -4100,7 +4100,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -4108,10 +4108,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -4119,10 +4119,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -4130,10 +4130,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -4141,10 +4141,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -4152,10 +4152,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -4163,10 +4163,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -4174,10 +4174,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -4185,10 +4185,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -4196,10 +4196,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -4207,10 +4207,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -4218,10 +4218,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -4229,10 +4229,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -4240,10 +4240,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -4251,10 +4251,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -4262,10 +4262,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -4273,10 +4273,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -4284,10 +4284,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -4295,10 +4295,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C21" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -4306,10 +4306,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -4317,10 +4317,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C23" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -4328,10 +4328,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -4339,10 +4339,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C25" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -4350,10 +4350,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -4361,10 +4361,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C27" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -4372,10 +4372,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -4383,10 +4383,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C29" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -4394,10 +4394,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -4405,10 +4405,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -4416,10 +4416,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C32" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -4427,10 +4427,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C33" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -4438,10 +4438,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C34" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -4449,10 +4449,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C35" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -4460,10 +4460,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C36" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update coordinates that prof didn't supply
</commit_message>
<xml_diff>
--- a/bus_stops.xlsx
+++ b/bus_stops.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seankzw/Desktop/SIT/Y1T2/csc1108/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFE9224-1F3F-D645-9CEA-0E13E8B2C252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAF1CCA-4973-8D49-9915-2DF317DA22A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F10A9419-1CB3-714B-AE05-C7B58E3111EF}"/>
+    <workbookView xWindow="8400" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F10A9419-1CB3-714B-AE05-C7B58E3111EF}"/>
   </bookViews>
   <sheets>
     <sheet name="P101-loop" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="344">
   <si>
     <t>Bus stop</t>
   </si>
@@ -1079,23 +1079,40 @@
     <t>Taman Mewah</t>
   </si>
   <si>
-    <t>0,0</t>
-  </si>
-  <si>
     <t>Maktab Sultan Abu Bakar (English College)</t>
+  </si>
+  <si>
+    <t>1.514385, 103.634502</t>
+  </si>
+  <si>
+    <t>1.512786, 103.634445</t>
+  </si>
+  <si>
+    <t>1.522586, 103.679608</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1118,8 +1135,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1437,7 +1456,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1517,7 +1536,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -2671,7 +2690,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2753,8 +2772,8 @@
       <c r="B7" t="s">
         <v>137</v>
       </c>
-      <c r="C7" t="s">
-        <v>340</v>
+      <c r="C7" s="1" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2764,8 +2783,8 @@
       <c r="B8" t="s">
         <v>136</v>
       </c>
-      <c r="C8" t="s">
-        <v>340</v>
+      <c r="C8" s="2" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -3191,8 +3210,8 @@
       <c r="B14" t="s">
         <v>203</v>
       </c>
-      <c r="C14" t="s">
-        <v>340</v>
+      <c r="C14" s="1" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -3689,7 +3708,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3903,8 +3922,8 @@
       <c r="B19" t="s">
         <v>203</v>
       </c>
-      <c r="C19" t="s">
-        <v>340</v>
+      <c r="C19" s="1" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>